<commit_message>
UBC name changed. 화이팅이다. 철우야.
</commit_message>
<xml_diff>
--- a/summary - 복사본.xlsx
+++ b/summary - 복사본.xlsx
@@ -488,11 +488,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>gmail address
-Nimama2012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gmail
 Nimama2011</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -639,10 +634,6 @@
       </rPr>
       <t>(Pratt)  spring ms only</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(+82)-010-8301-0173</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1043,7 +1034,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UBritishC
+    <t>gmail address
+Nimama2012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(+82)-010-8301-0173</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UBC
 deadline물어보기.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1677,8 +1677,8 @@
   <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1721,7 +1721,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
@@ -1729,22 +1729,22 @@
         <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1756,27 +1756,27 @@
         <v>130</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>128</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>
@@ -1784,13 +1784,13 @@
     </row>
     <row r="7" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
@@ -1802,13 +1802,13 @@
     </row>
     <row r="8" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1821,27 +1821,27 @@
     </row>
     <row r="10" spans="1:9" s="16" customFormat="1" ht="120.75" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>53</v>
@@ -1876,7 +1876,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1900,48 +1900,48 @@
     </row>
     <row r="71" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C71" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="H71" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="99" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2347,7 +2347,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2359,18 +2359,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2378,45 +2378,45 @@
         <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F7">
         <v>100081</v>
@@ -2424,73 +2424,73 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="181.5" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update. d-1 day. santa cruz
</commit_message>
<xml_diff>
--- a/summary - 복사본.xlsx
+++ b/summary - 복사본.xlsx
@@ -1247,30 +1247,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cs:http://ga.soe.ucsc.edu/admissions
-https://apply.embark.com/Grad/UCSantaCruz/83/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">page9,10,
-얘네들 대학에서 배운 지식으로 어떻게 다른 사람 도울것인지 쓰래..
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>statement of purpose,안썻으.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">last name과 firstname 바뀜 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1364,6 +1340,56 @@
     <t>cs:http://www.cise.ufl.edu/admissions/grad/apply.html
 신청페이지 시간 제한 있으. 
 https://www.isis.ufl.edu/cgi-bin/eaglec?page=IGA-INTRO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">page9,10,
+얘네들 대학에서 배운 지식으로 어떻게 다른 사람 도울것인지 쓰래..
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">statement of purpose,안썻으.
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cs:http://ga.soe.ucsc.edu/admissions
+https://apply.embark.com/Grad/UCSantaCruz/83/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>여기 장학금정보 꼭 보기.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+http://graddiv.ucsc.edu/prospective-students/application-filing-requirements/online-app-instructions.html</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2157,6 +2183,9 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2198,9 +2227,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2575,8 +2601,8 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2662,7 +2688,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="D5" s="57" t="s">
         <v>166</v>
@@ -2674,7 +2700,7 @@
         <v>174</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="66" x14ac:dyDescent="0.3">
@@ -2685,16 +2711,16 @@
         <v>148</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F6" s="73" t="s">
-        <v>177</v>
+      <c r="F6" s="59" t="s">
+        <v>175</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" ht="103.5" x14ac:dyDescent="0.3">
@@ -2731,7 +2757,7 @@
         <v>133</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>106</v>
@@ -2749,13 +2775,13 @@
         <v>144</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>170</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="66" x14ac:dyDescent="0.3">
@@ -2766,7 +2792,7 @@
         <v>149</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>135</v>
@@ -3463,93 +3489,93 @@
       <c r="A12" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="67" t="s">
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="67" t="s">
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="K12" s="69"/>
+      <c r="K12" s="70"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="41"/>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="71"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="37" t="s">
         <v>119</v>
       </c>
       <c r="E13" s="36"/>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="71" t="s">
         <v>118</v>
       </c>
-      <c r="G13" s="71"/>
+      <c r="G13" s="72"/>
       <c r="H13" s="37" t="s">
         <v>119</v>
       </c>
       <c r="I13" s="36"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="72"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="73"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
-      <c r="B14" s="61" t="s">
+      <c r="A14" s="64"/>
+      <c r="B14" s="62" t="s">
         <v>120</v>
       </c>
       <c r="C14" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="61" t="s">
+      <c r="F14" s="62" t="s">
         <v>120</v>
       </c>
       <c r="G14" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="H14" s="65" t="s">
+      <c r="H14" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="J14" s="61" t="s">
+      <c r="J14" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="K14" s="59" t="s">
+      <c r="K14" s="60" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="64"/>
-      <c r="B15" s="62"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="63"/>
       <c r="C15" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="62"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="63"/>
       <c r="G15" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="H15" s="66"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="60"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="61"/>
     </row>
     <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="42">

</xml_diff>

<commit_message>
alberta, duke를 추가 완성 하자.
</commit_message>
<xml_diff>
--- a/summary - 복사본.xlsx
+++ b/summary - 복사본.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="172">
   <si>
     <t>Univ</t>
   </si>
@@ -471,11 +471,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">2JW77N8Q849
-Nimama2011 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ronald Parr, Carlo Tomasi, Vincent Conit</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -490,13 +485,6 @@
 grad-info@cs.purdue.edu
 cs homepage:
 http://www.cs.purdue.edu/academic_programs/graduate/admission/steps.sxhtml</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intro
-http://www.cs.duke.edu/education/graduate/prospective/resources
-신청:
-https://app.applyyourself.com/?id=DukeGrad</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1017,10 +1005,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>신청 시스템에 계정 개설 안된다..</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.applyweb.com/cgi-bin/ustat?formcode=osugrad</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1113,20 +1097,6 @@
       <t xml:space="preserve">statement of purpose,안썻으.
 </t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">cs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions
-https://www.gradbase.ualberta.ca/sso/pages/login.jsp
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>추천서가 2개는 교수한테서 와야된다, 그래서 메일써 문의함.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">접촉한 선생의 이름 쓰란다. 흑인 이름써. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1284,12 +1254,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>두개의  noline system 에서 동시에 신청 해야된다. !
-GRE institution code - 0982 Department code - 0402
-TOEFL Institution code - 0982  Department Code - 78</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>https://apply.sgs.utoronto.ca/
 201208187329  Nimama2011
@@ -1310,12 +1274,56 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Waterloo??</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>university of alberta
 UW와 바꿀가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Waterloo??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T/G code 5812
+TG sent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>접촉한 선생의 이름 쓰란다. 흑인 이름써. 
+T/G 1592
+TG sent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6609 T/G
+TG sent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>두개의  noline system 에서 동시에 신청 해야된다. !
+TG sent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intro
+http://www.cs.duke.edu/education/graduate/prospective/resources
+신청:
+https://app.applyyourself.com/?id=DukeGrad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2JW77N8Q849
+Nimama2011 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">cs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions
+docs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions/required-documents
+https://www.gradbase.ualberta.ca/sso/pages/login.jsp
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAP 라는 시스템에서 계정 다시 만들고 시작해야돼.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2167,6 +2175,66 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2190,66 +2258,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2556,8 +2564,8 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2579,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>5</v>
@@ -2591,7 +2599,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -2605,104 +2613,107 @@
     </row>
     <row r="2" spans="1:9" s="33" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="32" t="s">
+    </row>
+    <row r="4" spans="1:9" s="58" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="58" t="s">
         <v>149</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="72" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="69" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="H4" s="72" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="H6" s="79" t="s">
-        <v>166</v>
+      <c r="H6" s="65" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="66" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="78" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="I8" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="13" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2711,44 +2722,45 @@
     </row>
     <row r="11" spans="1:9" s="13" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="13" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="13" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B13" s="48">
         <v>41289</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="F13" s="77" t="s">
-        <v>154</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="F13" s="63"/>
       <c r="H13" s="53" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
-        <v>169</v>
+      <c r="A14" s="67" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="17.25" x14ac:dyDescent="0.2">
@@ -2756,35 +2768,35 @@
       <c r="B16" s="24"/>
     </row>
     <row r="18" spans="1:8" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="75" t="s">
-        <v>147</v>
+      <c r="A18" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>144</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="7" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="73" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" s="76"/>
+      <c r="A19" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="62"/>
       <c r="D19" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -2793,13 +2805,13 @@
     </row>
     <row r="21" spans="1:8" s="33" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="51" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2827,10 +2839,10 @@
         <v>39</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>41</v>
@@ -2850,10 +2862,10 @@
         <v>37</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>57</v>
@@ -2862,27 +2874,27 @@
         <v>46</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="26" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="C73" s="80" t="s">
+        <v>157</v>
+      </c>
+      <c r="C73" s="66" t="s">
         <v>54</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E73" s="26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F73" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H73" s="26" t="s">
         <v>38</v>
@@ -2954,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -2983,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
@@ -3035,7 +3047,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -3064,7 +3076,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
@@ -3118,7 +3130,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
@@ -3145,7 +3157,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
@@ -3172,7 +3184,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
@@ -3319,7 +3331,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3327,25 +3339,25 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
         <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3355,33 +3367,33 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="43" t="s">
+      <c r="E10" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="F10" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="G10" s="43" t="s">
         <v>109</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="43" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C11" s="44">
         <v>28</v>
@@ -3401,95 +3413,95 @@
     </row>
     <row r="12" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="62" t="s">
-        <v>98</v>
-      </c>
-      <c r="K12" s="64"/>
+      <c r="K12" s="70"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="39"/>
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="72"/>
+      <c r="D13" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="34"/>
+      <c r="F13" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="72"/>
+      <c r="H13" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="73"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="78"/>
+      <c r="B14" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="35" t="s">
+      <c r="C14" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="65" t="s">
+      <c r="D14" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="35" t="s">
+      <c r="E14" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="67"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="58"/>
-      <c r="B14" s="56" t="s">
+      <c r="H14" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="K14" s="74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="79"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="60" t="s">
+      <c r="D15" s="81"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="E14" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="60" t="s">
-        <v>101</v>
-      </c>
-      <c r="I14" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="J14" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14" s="54" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="59"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="55"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="75"/>
     </row>
     <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="40">
@@ -3539,7 +3551,7 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
@@ -3549,12 +3561,12 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
@@ -3574,7 +3586,7 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
@@ -3604,17 +3616,17 @@
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
@@ -3624,17 +3636,17 @@
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
@@ -3644,17 +3656,11 @@
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
@@ -3664,6 +3670,12 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H14:H15"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
use this for ETS scholar ship.
</commit_message>
<xml_diff>
--- a/summary - 복사본.xlsx
+++ b/summary - 복사본.xlsx
@@ -1311,6 +1311,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">cs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions
+docs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions/required-documents
+https://gaps.cs.ualberta.ca/
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>https://apply.sgs.utoronto.ca/
 201208187329  Nimama2011
@@ -1329,13 +1336,6 @@
       <t>거의 완성
 https://gradapps.cs.toronto.edu/~mscac13/apply?loginKey=YAFBF0UMIFSNHRZ4Z5R77FRM325V9N07</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">cs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions
-docs:https://www.cs.ualberta.ca/prospective-students/graduate-studies/applications-admissions/required-documents
-https://gaps.cs.ualberta.ca/
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2245,6 +2245,24 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2267,24 +2285,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2660,8 +2660,8 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2758,7 +2758,7 @@
         <v>121</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>160</v>
@@ -2858,7 +2858,7 @@
         <v>41289</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>165</v>
@@ -3533,93 +3533,93 @@
       <c r="A12" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="79" t="s">
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="79" t="s">
+      <c r="G12" s="72"/>
+      <c r="H12" s="72"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="81"/>
+      <c r="K12" s="73"/>
     </row>
     <row r="13" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38"/>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="34" t="s">
         <v>95</v>
       </c>
       <c r="E13" s="33"/>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="83"/>
+      <c r="G13" s="75"/>
       <c r="H13" s="34" t="s">
         <v>95</v>
       </c>
       <c r="I13" s="33"/>
-      <c r="J13" s="82"/>
-      <c r="K13" s="84"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="76"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="81"/>
+      <c r="B14" s="79" t="s">
         <v>96</v>
       </c>
       <c r="C14" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="77" t="s">
+      <c r="D14" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="F14" s="79" t="s">
         <v>96</v>
       </c>
       <c r="G14" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="77" t="s">
+      <c r="H14" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="71" t="s">
+      <c r="I14" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="J14" s="73" t="s">
+      <c r="J14" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="K14" s="71" t="s">
+      <c r="K14" s="77" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="76"/>
-      <c r="B15" s="74"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="78"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="74"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="80"/>
       <c r="G15" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="H15" s="78"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="72"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="78"/>
     </row>
     <row r="16" spans="1:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="39">
@@ -3779,12 +3779,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
@@ -3794,6 +3788,12 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="H14:H15"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>